<commit_message>
Added two columns to spreadsheet.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81065589-F794-4C50-A54E-E025B7E4FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC0D8587-BF42-4EE2-AB19-61086192B6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="22380" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Height</t>
   </si>
@@ -99,6 +99,24 @@
   </si>
   <si>
     <t>white</t>
+  </si>
+  <si>
+    <t>HS Graduate</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -142,9 +160,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,264 +449,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>180</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>81</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>175</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>74</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>60</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>178</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>192</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>95</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>89</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>156</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>90</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>166</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>155</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>73</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>145</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>7000</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>49</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="F11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>165</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>53</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="F12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>133</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="F13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>166</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>52</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>154</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>50</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>65</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="3">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -698,14 +821,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -727,7 +850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -738,7 +861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Performed analysis code, eda code, processing code, and starter analysis report
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81065589-F794-4C50-A54E-E025B7E4FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C66815-8CBA-412A-A6B1-909F03A44045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="22380" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -428,12 +428,19 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
@@ -467,7 +474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
@@ -484,7 +491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -501,7 +508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -518,7 +525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
@@ -535,7 +542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -552,7 +559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
@@ -569,7 +576,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
@@ -586,7 +593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
@@ -603,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
@@ -620,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
@@ -634,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
@@ -651,7 +658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
@@ -668,7 +675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
@@ -698,14 +705,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -727,7 +734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -738,7 +745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Updated code to work with my two columns added to the spreadsheet
named them all with a 3 at the end
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21BBB946-9741-4C37-8450-19929E1E8EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA070AC-C081-4069-A8B3-1A2A9DA43EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1290" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Height</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>HS Graduate</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>Yes</t>
@@ -416,7 +413,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +449,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,7 +466,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,7 +483,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,7 +500,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,7 +517,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,7 +534,7 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,7 +551,7 @@
         <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,7 +568,7 @@
         <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,7 +585,7 @@
         <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -605,7 +602,7 @@
         <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,8 +612,8 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
+      <c r="D12">
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -636,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -653,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -670,7 +667,7 @@
         <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>